<commit_message>
functional refactoring of unexpectedResults
</commit_message>
<xml_diff>
--- a/dmn-excel-tester/src/test/resources/collect/beveragesExpected.xlsx
+++ b/dmn-excel-tester/src/test/resources/collect/beveragesExpected.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811B45D1-5080-4D3F-9CFE-9872297C1C7D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Dish</t>
   </si>
@@ -46,12 +47,18 @@
   </si>
   <si>
     <t>Unknown Dish</t>
+  </si>
+  <si>
+    <t>Steak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinot Noir; Water; Apple Juice; Gin; Whiskey </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,15 +369,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -408,6 +416,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>